<commit_message>
Setup dimension calculations and reading the sheet.
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Docs\code\ChristmasDrawing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3B8236-5DA8-4589-84B6-6BCFF71DB179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734CF90D-5E4C-4DF6-B5C7-12FB77747A1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{438FFFB8-2CEE-45FC-929D-C98E93549360}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>